<commit_message>
getDelta is now working, takes dataframe as input
</commit_message>
<xml_diff>
--- a/test/Sample data/PatientOverview_test.xlsx
+++ b/test/Sample data/PatientOverview_test.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="14">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="16">
   <si>
     <t>Antal</t>
   </si>
@@ -66,6 +66,12 @@
   </si>
   <si>
     <t>Consultation</t>
+  </si>
+  <si>
+    <t>Marfan</t>
+  </si>
+  <si>
+    <t>DQ874</t>
   </si>
 </sst>
 </file>
@@ -127,7 +133,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="7">
+  <borders count="8">
     <border>
       <left/>
       <right/>
@@ -199,11 +205,22 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="25">
+  <cellXfs count="29">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
@@ -275,6 +292,18 @@
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -560,7 +589,7 @@
   <dimension ref="A1:L23"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G2" sqref="G2"/>
+      <selection activeCell="G19" sqref="G19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.05" x14ac:dyDescent="0.3"/>
@@ -617,7 +646,7 @@
       <c r="D2" s="7"/>
       <c r="E2" s="7"/>
       <c r="F2" s="8">
-        <v>11</v>
+        <v>5</v>
       </c>
       <c r="G2" s="9">
         <v>1</v>
@@ -633,17 +662,31 @@
       <c r="L2" s="4"/>
     </row>
     <row r="3" spans="1:12" ht="15.65" x14ac:dyDescent="0.3">
-      <c r="A3" s="11"/>
-      <c r="B3" s="12"/>
-      <c r="C3" s="12"/>
-      <c r="D3" s="13"/>
-      <c r="E3" s="13"/>
-      <c r="F3" s="14"/>
-      <c r="G3" s="15"/>
-      <c r="H3" s="13"/>
-      <c r="I3" s="15"/>
-      <c r="J3" s="15"/>
-      <c r="K3" s="13"/>
+      <c r="A3" s="5" t="s">
+        <v>14</v>
+      </c>
+      <c r="B3" s="25" t="s">
+        <v>15</v>
+      </c>
+      <c r="C3" s="26"/>
+      <c r="D3" s="26"/>
+      <c r="E3" s="26"/>
+      <c r="F3" s="27">
+        <v>10</v>
+      </c>
+      <c r="G3" s="28">
+        <v>1</v>
+      </c>
+      <c r="H3" s="28"/>
+      <c r="I3" s="28">
+        <v>1</v>
+      </c>
+      <c r="J3" s="28">
+        <v>1</v>
+      </c>
+      <c r="K3" s="28">
+        <v>1</v>
+      </c>
       <c r="L3" s="16"/>
     </row>
     <row r="4" spans="1:12" ht="15.65" x14ac:dyDescent="0.3">
@@ -933,6 +976,21 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement/>
+</p:properties>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Dokument" ma:contentTypeID="0x0101004792E0B1DD728F47A9D3A151D94C43C2" ma:contentTypeVersion="2" ma:contentTypeDescription="Opret et nyt dokument." ma:contentTypeScope="" ma:versionID="8cbc72be1ef08462ba104cabf918da17">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns3="6edaa03f-8cd3-4dde-a2dc-6fcdfb7e57e2" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="6559be5467c1c92e09b21fd7a0e33ede" ns3:_="">
     <xsd:import namespace="6edaa03f-8cd3-4dde-a2dc-6fcdfb7e57e2"/>
@@ -1064,22 +1122,31 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
+<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{914321DA-A335-46C2-A508-540C232B6506}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="6edaa03f-8cd3-4dde-a2dc-6fcdfb7e57e2"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement/>
-</p:properties>
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{DC205DAF-0ED0-463C-A893-F538582E6260}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
-<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{224EDE6B-EE16-49F6-B299-4BBB0740FE85}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -1095,28 +1162,4 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{DC205DAF-0ED0-463C-A893-F538582E6260}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{914321DA-A335-46C2-A508-540C232B6506}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="6edaa03f-8cd3-4dde-a2dc-6fcdfb7e57e2"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
Will only solve the same type of suproblem once
</commit_message>
<xml_diff>
--- a/test/Sample data/PatientOverview_test.xlsx
+++ b/test/Sample data/PatientOverview_test.xlsx
@@ -589,7 +589,7 @@
   <dimension ref="A1:L23"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G19" sqref="G19"/>
+      <selection activeCell="J7" sqref="J7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.05" x14ac:dyDescent="0.3"/>
@@ -646,7 +646,7 @@
       <c r="D2" s="7"/>
       <c r="E2" s="7"/>
       <c r="F2" s="8">
-        <v>5</v>
+        <v>10</v>
       </c>
       <c r="G2" s="9">
         <v>1</v>

</xml_diff>

<commit_message>
Data can now be written and read to CSV files
</commit_message>
<xml_diff>
--- a/test/Sample data/PatientOverview_test.xlsx
+++ b/test/Sample data/PatientOverview_test.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="24042" windowHeight="9742"/>
+    <workbookView minimized="1" xWindow="0" yWindow="0" windowWidth="24042" windowHeight="9742"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -607,7 +607,7 @@
   <dimension ref="A1:L23"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="M1" sqref="M1"/>
+      <selection activeCell="H8" sqref="H8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.05" x14ac:dyDescent="0.3"/>
@@ -731,9 +731,7 @@
       <c r="I4" s="28">
         <v>1</v>
       </c>
-      <c r="J4" s="28">
-        <v>0</v>
-      </c>
+      <c r="J4" s="28"/>
       <c r="K4" s="13"/>
       <c r="L4" s="16"/>
     </row>
@@ -753,15 +751,11 @@
       <c r="G5" s="28">
         <v>1</v>
       </c>
-      <c r="H5" s="28">
-        <v>0</v>
-      </c>
+      <c r="H5" s="28"/>
       <c r="I5" s="28">
         <v>1</v>
       </c>
-      <c r="J5" s="28">
-        <v>0</v>
-      </c>
+      <c r="J5" s="28"/>
       <c r="K5" s="28">
         <v>1</v>
       </c>
@@ -1026,6 +1020,21 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement/>
+</p:properties>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Dokument" ma:contentTypeID="0x0101004792E0B1DD728F47A9D3A151D94C43C2" ma:contentTypeVersion="2" ma:contentTypeDescription="Opret et nyt dokument." ma:contentTypeScope="" ma:versionID="8cbc72be1ef08462ba104cabf918da17">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns3="6edaa03f-8cd3-4dde-a2dc-6fcdfb7e57e2" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="6559be5467c1c92e09b21fd7a0e33ede" ns3:_="">
     <xsd:import namespace="6edaa03f-8cd3-4dde-a2dc-6fcdfb7e57e2"/>
@@ -1157,22 +1166,31 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
+<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{914321DA-A335-46C2-A508-540C232B6506}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="6edaa03f-8cd3-4dde-a2dc-6fcdfb7e57e2"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement/>
-</p:properties>
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{DC205DAF-0ED0-463C-A893-F538582E6260}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
-<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{224EDE6B-EE16-49F6-B299-4BBB0740FE85}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -1188,28 +1206,4 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{DC205DAF-0ED0-463C-A893-F538582E6260}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{914321DA-A335-46C2-A508-540C232B6506}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="6edaa03f-8cd3-4dde-a2dc-6fcdfb7e57e2"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
 </file>
</xml_diff>